<commit_message>
interview 3 chart and data path
</commit_message>
<xml_diff>
--- a/Interviews_Columns/Interview 3.xlsx
+++ b/Interviews_Columns/Interview 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pzban\Documents\GitHub\PROJECT-E4\Interviews_Columns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:400001_{E800629A-5CFC-42EF-87C0-F930BE42FF48}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:400001_{69BC1383-2851-4050-8404-D9F295002C14}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>table: student</t>
   </si>
@@ -63,22 +63,10 @@
     <t>difficulty index</t>
   </si>
   <si>
-    <t>student type</t>
-  </si>
-  <si>
-    <t>char</t>
-  </si>
-  <si>
-    <t>students' type A, B, C......</t>
-  </si>
-  <si>
     <t>difficulty</t>
   </si>
   <si>
     <t>student who are in difficulty</t>
-  </si>
-  <si>
-    <t>spend time per week</t>
   </si>
   <si>
     <t>pass rate</t>
@@ -530,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -543,6 +531,7 @@
     <col min="3" max="3" width="32.5546875" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -550,24 +539,24 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>4</v>
@@ -584,10 +573,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -601,21 +590,21 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -626,13 +615,13 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -643,24 +632,24 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -679,75 +668,56 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="C16" s="1" t="s">
-        <v>30</v>
+      <c r="C16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3">
-      <c r="C21" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3">
-      <c r="C22" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>